<commit_message>
Change template 3g file with 3 ranges
</commit_message>
<xml_diff>
--- a/output/template_single_3g.xlsx
+++ b/output/template_single_3g.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diuoagr-my.sharepoint.com/personal/grad0909_di_uoa_gr/Documents/Surecom/Surecom_KPI/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1B8E7F04-2C69-4B04-8A8E-FE09789561F9}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EC12CFC-C9A4-45F3-AEE5-6C26AC45E9D3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input3G" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>UMTS RSCP (dBm)</t>
   </si>
@@ -43,63 +50,18 @@
     <t xml:space="preserve">Serving </t>
   </si>
   <si>
-    <t>-90 to -85</t>
-  </si>
-  <si>
-    <t>-85 to -80</t>
-  </si>
-  <si>
-    <t>-80 to -75</t>
-  </si>
-  <si>
-    <t>-75 to -70</t>
-  </si>
-  <si>
     <t>&lt;= -13</t>
   </si>
   <si>
     <t>-13 to -10</t>
   </si>
   <si>
-    <t>-10 to -7</t>
-  </si>
-  <si>
-    <t>-7 to -4</t>
-  </si>
-  <si>
-    <t>&gt;= -4</t>
-  </si>
-  <si>
-    <t>-34 to -13</t>
-  </si>
-  <si>
-    <t>-4 to 0</t>
-  </si>
-  <si>
-    <t>&lt;= -90</t>
-  </si>
-  <si>
-    <t>-70 to -65</t>
-  </si>
-  <si>
-    <t>-65 to -60</t>
-  </si>
-  <si>
-    <t>-60 to -55</t>
-  </si>
-  <si>
-    <t>&gt;= -55</t>
-  </si>
-  <si>
     <t>UARFCN</t>
   </si>
   <si>
     <t>SC</t>
   </si>
   <si>
-    <t>-55 to -15</t>
-  </si>
-  <si>
     <t>UMTS UARFCN</t>
   </si>
   <si>
@@ -112,10 +74,28 @@
     <t>sc</t>
   </si>
   <si>
-    <t>Eir:input\EIR F-4 U21.FMT</t>
-  </si>
-  <si>
     <t>UMTS Ec/No (dB)</t>
+  </si>
+  <si>
+    <t>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</t>
+  </si>
+  <si>
+    <t>&lt;= -101</t>
+  </si>
+  <si>
+    <t>-101 to -94</t>
+  </si>
+  <si>
+    <t>-94 to -15</t>
+  </si>
+  <si>
+    <t>-34 to -15</t>
+  </si>
+  <si>
+    <t>-15 to 0</t>
+  </si>
+  <si>
+    <t>&gt;= -94</t>
   </si>
 </sst>
 </file>
@@ -168,7 +148,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,50 +169,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF48F836"/>
+        <fgColor theme="9"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF33CC33"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF006600"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF44546A"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -356,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -377,10 +327,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -393,60 +339,47 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,17 +661,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C30"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -748,122 +681,99 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>3156</v>
+        <v>1375</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>1.1678075792835099E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1429</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.21367056785174E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>114938</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
+        <v>0.97618521852864704</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>6855</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>5.82205160435528E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>110887</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
+        <v>0.94177948395644695</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13">
+        <v>2962</v>
+      </c>
+      <c r="B13">
+        <v>117742</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
+      <c r="A14">
+        <v>10637</v>
       </c>
       <c r="B14">
-        <v>3156</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
+      <c r="A15">
+        <v>10662</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -873,122 +783,35 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
+      <c r="A16">
+        <v>10687</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2962</v>
-      </c>
-      <c r="B22">
-        <v>115</v>
-      </c>
-      <c r="C22">
-        <v>3.64385297845373E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>10637</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>10662</v>
-      </c>
-      <c r="B24">
-        <v>3041</v>
-      </c>
-      <c r="C24">
-        <v>0.96356147021546201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>10687</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>198</v>
-      </c>
-      <c r="B29">
-        <v>115</v>
-      </c>
-      <c r="C29">
-        <v>3.64385297845373E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>295</v>
-      </c>
-      <c r="B30">
-        <v>3041</v>
-      </c>
-      <c r="C30">
-        <v>0.96356147021546201</v>
+      <c r="A20">
+        <v>149</v>
+      </c>
+      <c r="B20">
+        <v>117742</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -998,10 +821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC13D29-B219-4AE5-9192-3696E6318D31}">
-  <dimension ref="B2:D69"/>
+  <dimension ref="B2:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,271 +835,290 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="26"/>
+      <c r="B2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15"/>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11">
+        <f>Input3G!C3</f>
+        <v>1.1678075792835099E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15">
-        <f>Input3G!C3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="15">
+      <c r="C4" s="13"/>
+      <c r="D4" s="11">
         <f>Input3G!C4</f>
-        <v>0</v>
+        <v>1.21367056785174E-2</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="11">
+        <f>Input3G!C5</f>
+        <v>0.97618521852864704</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="str">
+        <f>Input3G!A1</f>
+        <v>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="1">
+        <f>Input3G!C8</f>
+        <v>5.82205160435528E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="15">
-        <f>Input3G!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="1">
+        <f>Input3G!C9</f>
+        <v>0.94177948395644695</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="str">
+        <f>Input3G!A1</f>
+        <v>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="22" t="str">
+        <f>Input3G!A1</f>
+        <v>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="26"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="15">
-        <f>Input3G!C6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="26"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <f>Input3G!A13</f>
+        <v>2962</v>
+      </c>
+      <c r="C15" s="1">
+        <f>Input3G!C13</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="26"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <f>Input3G!A14</f>
+        <v>10637</v>
+      </c>
+      <c r="C16" s="1">
+        <f>Input3G!C14</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <f>Input3G!A15</f>
+        <v>10662</v>
+      </c>
+      <c r="C17" s="1">
+        <f>Input3G!C15</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <f>Input3G!A16</f>
+        <v>10687</v>
+      </c>
+      <c r="C18" s="1">
+        <f>Input3G!C16</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="26"/>
+    </row>
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="22" t="str">
+        <f>Input3G!A1</f>
+        <v>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="26"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="15">
-        <f>Input3G!C7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="15">
-        <f>Input3G!C8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="15">
-        <f>Input3G!C9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="15">
-        <f>Input3G!C10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="15">
-        <f>Input3G!C11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="str">
-        <f>Input3G!A1</f>
-        <v>Eir:input\EIR F-4 U21.FMT</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-    </row>
-    <row r="14" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="1">
-        <f>Input3G!C14</f>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="26"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9">
+        <f>Input3G!A20</f>
+        <v>149</v>
+      </c>
+      <c r="C22" s="1">
+        <f>Input3G!C20</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="1">
-        <f>Input3G!C15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="1">
-        <f>Input3G!C16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="1">
-        <f>Input3G!C17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="1">
-        <f>Input3G!C18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="str">
-        <f>Input3G!A1</f>
-        <v>Eir:input\EIR F-4 U21.FMT</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="32"/>
-    </row>
-    <row r="22" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="str">
-        <f>Input3G!A1</f>
-        <v>Eir:input\EIR F-4 U21.FMT</v>
-      </c>
-      <c r="C22" s="33"/>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B23" s="10">
+        <f>Input3G!A21</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <f>Input3G!C21</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="12">
+      <c r="B24" s="10">
         <f>Input3G!A22</f>
-        <v>2962</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
         <f>Input3G!C22</f>
-        <v>3.64385297845373E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="12">
+      <c r="B25" s="10">
         <f>Input3G!A23</f>
-        <v>10637</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1">
         <f>Input3G!C23</f>
         <v>0</v>
       </c>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="12">
+      <c r="B26" s="10">
         <f>Input3G!A24</f>
-        <v>10662</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
         <f>Input3G!C24</f>
-        <v>0.96356147021546201</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="12">
+      <c r="B27" s="10">
         <f>Input3G!A25</f>
-        <v>10687</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1">
         <f>Input3G!C25</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="str">
-        <f>Input3G!A1</f>
-        <v>Eir:input\EIR F-4 U21.FMT</v>
-      </c>
-      <c r="C29" s="33"/>
+      <c r="D27" s="26"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="10">
+        <f>Input3G!A26</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <f>Input3G!C26</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="10">
+        <f>Input3G!A27</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <f>Input3G!C27</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="26"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B30" s="10">
+        <f>Input3G!A28</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <f>Input3G!C28</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="26"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="13">
+      <c r="B31" s="10">
         <f>Input3G!A29</f>
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="C31" s="1">
         <f>Input3G!C29</f>
-        <v>3.64385297845373E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="14">
+      <c r="B32" s="10">
         <f>Input3G!A30</f>
-        <v>295</v>
+        <v>0</v>
       </c>
       <c r="C32" s="1">
         <f>Input3G!C30</f>
-        <v>0.96356147021546201</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="14">
+        <v>0</v>
+      </c>
+      <c r="D32" s="26"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="10">
         <f>Input3G!A31</f>
         <v>0</v>
       </c>
@@ -1284,9 +1126,10 @@
         <f>Input3G!C31</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="14">
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="10">
         <f>Input3G!A32</f>
         <v>0</v>
       </c>
@@ -1294,9 +1137,10 @@
         <f>Input3G!C32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="14">
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="10">
         <f>Input3G!A33</f>
         <v>0</v>
       </c>
@@ -1304,9 +1148,10 @@
         <f>Input3G!C33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="14">
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="10">
         <f>Input3G!A34</f>
         <v>0</v>
       </c>
@@ -1314,9 +1159,10 @@
         <f>Input3G!C34</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="14">
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="10">
         <f>Input3G!A35</f>
         <v>0</v>
       </c>
@@ -1324,9 +1170,10 @@
         <f>Input3G!C35</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="14">
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="10">
         <f>Input3G!A36</f>
         <v>0</v>
       </c>
@@ -1334,9 +1181,10 @@
         <f>Input3G!C36</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="14">
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="10">
         <f>Input3G!A37</f>
         <v>0</v>
       </c>
@@ -1344,9 +1192,10 @@
         <f>Input3G!C37</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="14">
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="10">
         <f>Input3G!A38</f>
         <v>0</v>
       </c>
@@ -1354,9 +1203,10 @@
         <f>Input3G!C38</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="14">
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="10">
         <f>Input3G!A39</f>
         <v>0</v>
       </c>
@@ -1364,9 +1214,10 @@
         <f>Input3G!C39</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="14">
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="10">
         <f>Input3G!A40</f>
         <v>0</v>
       </c>
@@ -1374,9 +1225,10 @@
         <f>Input3G!C40</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="14">
+      <c r="D42" s="26"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="10">
         <f>Input3G!A41</f>
         <v>0</v>
       </c>
@@ -1384,9 +1236,10 @@
         <f>Input3G!C41</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="14">
+      <c r="D43" s="26"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="10">
         <f>Input3G!A42</f>
         <v>0</v>
       </c>
@@ -1394,9 +1247,10 @@
         <f>Input3G!C42</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="14">
+      <c r="D44" s="26"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="10">
         <f>Input3G!A43</f>
         <v>0</v>
       </c>
@@ -1404,9 +1258,10 @@
         <f>Input3G!C43</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="14">
+      <c r="D45" s="26"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="10">
         <f>Input3G!A44</f>
         <v>0</v>
       </c>
@@ -1414,9 +1269,10 @@
         <f>Input3G!C44</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="14">
+      <c r="D46" s="26"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="10">
         <f>Input3G!A45</f>
         <v>0</v>
       </c>
@@ -1424,9 +1280,10 @@
         <f>Input3G!C45</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="14">
+      <c r="D47" s="26"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="10">
         <f>Input3G!A46</f>
         <v>0</v>
       </c>
@@ -1434,9 +1291,10 @@
         <f>Input3G!C46</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="14">
+      <c r="D48" s="26"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="10">
         <f>Input3G!A47</f>
         <v>0</v>
       </c>
@@ -1444,9 +1302,10 @@
         <f>Input3G!C47</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="14">
+      <c r="D49" s="26"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="10">
         <f>Input3G!A48</f>
         <v>0</v>
       </c>
@@ -1454,9 +1313,10 @@
         <f>Input3G!C48</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="14">
+      <c r="D50" s="26"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="10">
         <f>Input3G!A49</f>
         <v>0</v>
       </c>
@@ -1464,9 +1324,10 @@
         <f>Input3G!C49</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="14">
+      <c r="D51" s="26"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="10">
         <f>Input3G!A50</f>
         <v>0</v>
       </c>
@@ -1474,9 +1335,10 @@
         <f>Input3G!C50</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="14">
+      <c r="D52" s="26"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="10">
         <f>Input3G!A51</f>
         <v>0</v>
       </c>
@@ -1484,9 +1346,10 @@
         <f>Input3G!C51</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="14">
+      <c r="D53" s="26"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="10">
         <f>Input3G!A52</f>
         <v>0</v>
       </c>
@@ -1494,9 +1357,10 @@
         <f>Input3G!C52</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="14">
+      <c r="D54" s="26"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="10">
         <f>Input3G!A53</f>
         <v>0</v>
       </c>
@@ -1504,9 +1368,10 @@
         <f>Input3G!C53</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="14">
+      <c r="D55" s="26"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="10">
         <f>Input3G!A54</f>
         <v>0</v>
       </c>
@@ -1514,9 +1379,10 @@
         <f>Input3G!C54</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="14">
+      <c r="D56" s="26"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="10">
         <f>Input3G!A55</f>
         <v>0</v>
       </c>
@@ -1524,9 +1390,10 @@
         <f>Input3G!C55</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="14">
+      <c r="D57" s="26"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="10">
         <f>Input3G!A56</f>
         <v>0</v>
       </c>
@@ -1534,9 +1401,10 @@
         <f>Input3G!C56</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="14">
+      <c r="D58" s="26"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="10">
         <f>Input3G!A57</f>
         <v>0</v>
       </c>
@@ -1544,9 +1412,10 @@
         <f>Input3G!C57</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="14">
+      <c r="D59" s="26"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="10">
         <f>Input3G!A58</f>
         <v>0</v>
       </c>
@@ -1554,96 +1423,7 @@
         <f>Input3G!C58</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="14">
-        <f>Input3G!A59</f>
-        <v>0</v>
-      </c>
-      <c r="C61" s="1">
-        <f>Input3G!C59</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="14">
-        <f>Input3G!A60</f>
-        <v>0</v>
-      </c>
-      <c r="C62" s="1">
-        <f>Input3G!C60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="14">
-        <f>Input3G!A61</f>
-        <v>0</v>
-      </c>
-      <c r="C63" s="1">
-        <f>Input3G!C61</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="14">
-        <f>Input3G!A62</f>
-        <v>0</v>
-      </c>
-      <c r="C64" s="1">
-        <f>Input3G!C62</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="14">
-        <f>Input3G!A63</f>
-        <v>0</v>
-      </c>
-      <c r="C65" s="1">
-        <f>Input3G!C63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="14">
-        <f>Input3G!A64</f>
-        <v>0</v>
-      </c>
-      <c r="C66" s="1">
-        <f>Input3G!C64</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="14">
-        <f>Input3G!A65</f>
-        <v>0</v>
-      </c>
-      <c r="C67" s="1">
-        <f>Input3G!C65</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="14">
-        <f>Input3G!A66</f>
-        <v>0</v>
-      </c>
-      <c r="C68" s="1">
-        <f>Input3G!C66</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="14">
-        <f>Input3G!A67</f>
-        <v>0</v>
-      </c>
-      <c r="C69" s="1">
-        <f>Input3G!C67</f>
-        <v>0</v>
-      </c>
+      <c r="D60" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change template 3g file and python file for 3 ranges
</commit_message>
<xml_diff>
--- a/output/template_single_3g.xlsx
+++ b/output/template_single_3g.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diuoagr-my.sharepoint.com/personal/grad0909_di_uoa_gr/Documents/Surecom/Surecom_KPI/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EC12CFC-C9A4-45F3-AEE5-6C26AC45E9D3}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CB89BF0-E8B8-4F23-8A87-7B2955DC2BF2}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input3G" sheetId="1" r:id="rId1"/>
@@ -50,12 +50,6 @@
     <t xml:space="preserve">Serving </t>
   </si>
   <si>
-    <t>&lt;= -13</t>
-  </si>
-  <si>
-    <t>-13 to -10</t>
-  </si>
-  <si>
     <t>UARFCN</t>
   </si>
   <si>
@@ -96,6 +90,12 @@
   </si>
   <si>
     <t>&gt;= -94</t>
+  </si>
+  <si>
+    <t>-34 to -14</t>
+  </si>
+  <si>
+    <t>-14 to 0</t>
   </si>
 </sst>
 </file>
@@ -315,9 +315,6 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -380,6 +377,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,7 +671,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1375</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1429</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>114938</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>6855</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>110887</v>
@@ -741,12 +741,12 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -795,12 +795,12 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,108 +835,108 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11">
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="10">
         <f>Input3G!C3</f>
         <v>1.1678075792835099E-2</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="11">
+      <c r="B4" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="10">
         <f>Input3G!C4</f>
         <v>1.21367056785174E-2</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="11">
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="10">
         <f>Input3G!C5</f>
         <v>0.97618521852864704</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="str">
+      <c r="B6" s="15" t="str">
         <f>Input3G!A1</f>
         <v>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7"/>
+      <c r="B9" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="1">
         <f>Input3G!C8</f>
         <v>5.82205160435528E-2</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="25"/>
+      <c r="B10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="24"/>
       <c r="D10" s="1">
         <f>Input3G!C9</f>
         <v>0.94177948395644695</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="str">
+      <c r="B11" s="15" t="str">
         <f>Input3G!A1</f>
         <v>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="21"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="str">
+      <c r="B13" s="21" t="str">
         <f>Input3G!A1</f>
         <v>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="26"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="25"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
-        <v>7</v>
+      <c r="B14" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="26"/>
+      <c r="D14" s="25"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <f>Input3G!A13</f>
         <v>2962</v>
       </c>
@@ -944,10 +944,10 @@
         <f>Input3G!C13</f>
         <v>1</v>
       </c>
-      <c r="D15" s="26"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <f>Input3G!A14</f>
         <v>10637</v>
       </c>
@@ -955,10 +955,10 @@
         <f>Input3G!C14</f>
         <v>0</v>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <f>Input3G!A15</f>
         <v>10662</v>
       </c>
@@ -966,10 +966,10 @@
         <f>Input3G!C15</f>
         <v>0</v>
       </c>
-      <c r="D17" s="26"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <f>Input3G!A16</f>
         <v>10687</v>
       </c>
@@ -977,27 +977,27 @@
         <f>Input3G!C16</f>
         <v>0</v>
       </c>
-      <c r="D18" s="26"/>
+      <c r="D18" s="25"/>
     </row>
     <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="str">
+      <c r="B20" s="21" t="str">
         <f>Input3G!A1</f>
         <v>Eir:input\UMTSBlockC2F20210924T144614Z.FMT</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="26"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="25"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>8</v>
+      <c r="B21" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="26"/>
+      <c r="D21" s="25"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="9">
+      <c r="B22" s="8">
         <f>Input3G!A20</f>
         <v>149</v>
       </c>
@@ -1005,10 +1005,10 @@
         <f>Input3G!C20</f>
         <v>1</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D22" s="25"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <f>Input3G!A21</f>
         <v>0</v>
       </c>
@@ -1016,10 +1016,10 @@
         <f>Input3G!C21</f>
         <v>0</v>
       </c>
-      <c r="D23" s="26"/>
+      <c r="D23" s="25"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <f>Input3G!A22</f>
         <v>0</v>
       </c>
@@ -1027,10 +1027,10 @@
         <f>Input3G!C22</f>
         <v>0</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="25"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <f>Input3G!A23</f>
         <v>0</v>
       </c>
@@ -1038,10 +1038,10 @@
         <f>Input3G!C23</f>
         <v>0</v>
       </c>
-      <c r="D25" s="26"/>
+      <c r="D25" s="25"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <f>Input3G!A24</f>
         <v>0</v>
       </c>
@@ -1049,10 +1049,10 @@
         <f>Input3G!C24</f>
         <v>0</v>
       </c>
-      <c r="D26" s="26"/>
+      <c r="D26" s="25"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="10">
+      <c r="B27" s="9">
         <f>Input3G!A25</f>
         <v>0</v>
       </c>
@@ -1060,10 +1060,10 @@
         <f>Input3G!C25</f>
         <v>0</v>
       </c>
-      <c r="D27" s="26"/>
+      <c r="D27" s="25"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <f>Input3G!A26</f>
         <v>0</v>
       </c>
@@ -1071,10 +1071,10 @@
         <f>Input3G!C26</f>
         <v>0</v>
       </c>
-      <c r="D28" s="26"/>
+      <c r="D28" s="25"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <f>Input3G!A27</f>
         <v>0</v>
       </c>
@@ -1082,10 +1082,10 @@
         <f>Input3G!C27</f>
         <v>0</v>
       </c>
-      <c r="D29" s="26"/>
+      <c r="D29" s="25"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <f>Input3G!A28</f>
         <v>0</v>
       </c>
@@ -1093,10 +1093,10 @@
         <f>Input3G!C28</f>
         <v>0</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="25"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <f>Input3G!A29</f>
         <v>0</v>
       </c>
@@ -1104,10 +1104,10 @@
         <f>Input3G!C29</f>
         <v>0</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="25"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="10">
+      <c r="B32" s="9">
         <f>Input3G!A30</f>
         <v>0</v>
       </c>
@@ -1115,10 +1115,10 @@
         <f>Input3G!C30</f>
         <v>0</v>
       </c>
-      <c r="D32" s="26"/>
+      <c r="D32" s="25"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="10">
+      <c r="B33" s="9">
         <f>Input3G!A31</f>
         <v>0</v>
       </c>
@@ -1126,10 +1126,10 @@
         <f>Input3G!C31</f>
         <v>0</v>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="25"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="10">
+      <c r="B34" s="9">
         <f>Input3G!A32</f>
         <v>0</v>
       </c>
@@ -1137,10 +1137,10 @@
         <f>Input3G!C32</f>
         <v>0</v>
       </c>
-      <c r="D34" s="26"/>
+      <c r="D34" s="25"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="10">
+      <c r="B35" s="9">
         <f>Input3G!A33</f>
         <v>0</v>
       </c>
@@ -1148,10 +1148,10 @@
         <f>Input3G!C33</f>
         <v>0</v>
       </c>
-      <c r="D35" s="26"/>
+      <c r="D35" s="25"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <f>Input3G!A34</f>
         <v>0</v>
       </c>
@@ -1159,10 +1159,10 @@
         <f>Input3G!C34</f>
         <v>0</v>
       </c>
-      <c r="D36" s="26"/>
+      <c r="D36" s="25"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="10">
+      <c r="B37" s="9">
         <f>Input3G!A35</f>
         <v>0</v>
       </c>
@@ -1170,10 +1170,10 @@
         <f>Input3G!C35</f>
         <v>0</v>
       </c>
-      <c r="D37" s="26"/>
+      <c r="D37" s="25"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="10">
+      <c r="B38" s="9">
         <f>Input3G!A36</f>
         <v>0</v>
       </c>
@@ -1181,10 +1181,10 @@
         <f>Input3G!C36</f>
         <v>0</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="25"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="10">
+      <c r="B39" s="9">
         <f>Input3G!A37</f>
         <v>0</v>
       </c>
@@ -1192,10 +1192,10 @@
         <f>Input3G!C37</f>
         <v>0</v>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="25"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="10">
+      <c r="B40" s="9">
         <f>Input3G!A38</f>
         <v>0</v>
       </c>
@@ -1203,10 +1203,10 @@
         <f>Input3G!C38</f>
         <v>0</v>
       </c>
-      <c r="D40" s="26"/>
+      <c r="D40" s="25"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="10">
+      <c r="B41" s="9">
         <f>Input3G!A39</f>
         <v>0</v>
       </c>
@@ -1214,10 +1214,10 @@
         <f>Input3G!C39</f>
         <v>0</v>
       </c>
-      <c r="D41" s="26"/>
+      <c r="D41" s="25"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="10">
+      <c r="B42" s="9">
         <f>Input3G!A40</f>
         <v>0</v>
       </c>
@@ -1225,10 +1225,10 @@
         <f>Input3G!C40</f>
         <v>0</v>
       </c>
-      <c r="D42" s="26"/>
+      <c r="D42" s="25"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="10">
+      <c r="B43" s="9">
         <f>Input3G!A41</f>
         <v>0</v>
       </c>
@@ -1236,10 +1236,10 @@
         <f>Input3G!C41</f>
         <v>0</v>
       </c>
-      <c r="D43" s="26"/>
+      <c r="D43" s="25"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="10">
+      <c r="B44" s="9">
         <f>Input3G!A42</f>
         <v>0</v>
       </c>
@@ -1247,10 +1247,10 @@
         <f>Input3G!C42</f>
         <v>0</v>
       </c>
-      <c r="D44" s="26"/>
+      <c r="D44" s="25"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="10">
+      <c r="B45" s="9">
         <f>Input3G!A43</f>
         <v>0</v>
       </c>
@@ -1258,10 +1258,10 @@
         <f>Input3G!C43</f>
         <v>0</v>
       </c>
-      <c r="D45" s="26"/>
+      <c r="D45" s="25"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="10">
+      <c r="B46" s="9">
         <f>Input3G!A44</f>
         <v>0</v>
       </c>
@@ -1269,10 +1269,10 @@
         <f>Input3G!C44</f>
         <v>0</v>
       </c>
-      <c r="D46" s="26"/>
+      <c r="D46" s="25"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <f>Input3G!A45</f>
         <v>0</v>
       </c>
@@ -1280,10 +1280,10 @@
         <f>Input3G!C45</f>
         <v>0</v>
       </c>
-      <c r="D47" s="26"/>
+      <c r="D47" s="25"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="10">
+      <c r="B48" s="9">
         <f>Input3G!A46</f>
         <v>0</v>
       </c>
@@ -1291,10 +1291,10 @@
         <f>Input3G!C46</f>
         <v>0</v>
       </c>
-      <c r="D48" s="26"/>
+      <c r="D48" s="25"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <f>Input3G!A47</f>
         <v>0</v>
       </c>
@@ -1302,10 +1302,10 @@
         <f>Input3G!C47</f>
         <v>0</v>
       </c>
-      <c r="D49" s="26"/>
+      <c r="D49" s="25"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="10">
+      <c r="B50" s="9">
         <f>Input3G!A48</f>
         <v>0</v>
       </c>
@@ -1313,10 +1313,10 @@
         <f>Input3G!C48</f>
         <v>0</v>
       </c>
-      <c r="D50" s="26"/>
+      <c r="D50" s="25"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="10">
+      <c r="B51" s="9">
         <f>Input3G!A49</f>
         <v>0</v>
       </c>
@@ -1324,10 +1324,10 @@
         <f>Input3G!C49</f>
         <v>0</v>
       </c>
-      <c r="D51" s="26"/>
+      <c r="D51" s="25"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="10">
+      <c r="B52" s="9">
         <f>Input3G!A50</f>
         <v>0</v>
       </c>
@@ -1335,10 +1335,10 @@
         <f>Input3G!C50</f>
         <v>0</v>
       </c>
-      <c r="D52" s="26"/>
+      <c r="D52" s="25"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="10">
+      <c r="B53" s="9">
         <f>Input3G!A51</f>
         <v>0</v>
       </c>
@@ -1346,10 +1346,10 @@
         <f>Input3G!C51</f>
         <v>0</v>
       </c>
-      <c r="D53" s="26"/>
+      <c r="D53" s="25"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="10">
+      <c r="B54" s="9">
         <f>Input3G!A52</f>
         <v>0</v>
       </c>
@@ -1357,10 +1357,10 @@
         <f>Input3G!C52</f>
         <v>0</v>
       </c>
-      <c r="D54" s="26"/>
+      <c r="D54" s="25"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="10">
+      <c r="B55" s="9">
         <f>Input3G!A53</f>
         <v>0</v>
       </c>
@@ -1368,10 +1368,10 @@
         <f>Input3G!C53</f>
         <v>0</v>
       </c>
-      <c r="D55" s="26"/>
+      <c r="D55" s="25"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="10">
+      <c r="B56" s="9">
         <f>Input3G!A54</f>
         <v>0</v>
       </c>
@@ -1379,10 +1379,10 @@
         <f>Input3G!C54</f>
         <v>0</v>
       </c>
-      <c r="D56" s="26"/>
+      <c r="D56" s="25"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="10">
+      <c r="B57" s="9">
         <f>Input3G!A55</f>
         <v>0</v>
       </c>
@@ -1390,10 +1390,10 @@
         <f>Input3G!C55</f>
         <v>0</v>
       </c>
-      <c r="D57" s="26"/>
+      <c r="D57" s="25"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="10">
+      <c r="B58" s="9">
         <f>Input3G!A56</f>
         <v>0</v>
       </c>
@@ -1401,10 +1401,10 @@
         <f>Input3G!C56</f>
         <v>0</v>
       </c>
-      <c r="D58" s="26"/>
+      <c r="D58" s="25"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="10">
+      <c r="B59" s="9">
         <f>Input3G!A57</f>
         <v>0</v>
       </c>
@@ -1412,10 +1412,10 @@
         <f>Input3G!C57</f>
         <v>0</v>
       </c>
-      <c r="D59" s="26"/>
+      <c r="D59" s="25"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="10">
+      <c r="B60" s="9">
         <f>Input3G!A58</f>
         <v>0</v>
       </c>
@@ -1423,7 +1423,7 @@
         <f>Input3G!C58</f>
         <v>0</v>
       </c>
-      <c r="D60" s="26"/>
+      <c r="D60" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>